<commit_message>
Migrated data to philippines_ff2.0_habitat
</commit_message>
<xml_diff>
--- a/src/data_migration/philippines/ff2.0/benthicpqt_mermaid_template.xlsx
+++ b/src/data_migration/philippines/ff2.0/benthicpqt_mermaid_template.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="946" uniqueCount="946">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="964" uniqueCount="964">
   <si>
     <t xml:space="preserve">Site *</t>
   </si>
@@ -556,6 +556,9 @@
     <t xml:space="preserve">Benthic attribute observed. See relevant tab on ingestion template for choices.</t>
   </si>
   <si>
+    <t xml:space="preserve">Abyla</t>
+  </si>
+  <si>
     <t xml:space="preserve">Acanthaster planci</t>
   </si>
   <si>
@@ -829,6 +832,9 @@
     <t xml:space="preserve">Asparagopsis taxiformis</t>
   </si>
   <si>
+    <t xml:space="preserve">Asteroidea</t>
+  </si>
+  <si>
     <t xml:space="preserve">Astraeosmilia</t>
   </si>
   <si>
@@ -919,9 +925,15 @@
     <t xml:space="preserve">Bonnemaisoniaceae</t>
   </si>
   <si>
+    <t xml:space="preserve">Boodlea</t>
+  </si>
+  <si>
     <t xml:space="preserve">Briareum</t>
   </si>
   <si>
+    <t xml:space="preserve">Bryopsis</t>
+  </si>
+  <si>
     <t xml:space="preserve">Bryozoan</t>
   </si>
   <si>
@@ -979,6 +991,9 @@
     <t xml:space="preserve">Chlorodesmis</t>
   </si>
   <si>
+    <t xml:space="preserve">Chlorophyta</t>
+  </si>
+  <si>
     <t xml:space="preserve">Chondrilla</t>
   </si>
   <si>
@@ -997,6 +1012,9 @@
     <t xml:space="preserve">Chrysocystis fragilis</t>
   </si>
   <si>
+    <t xml:space="preserve">Chrysophyceae</t>
+  </si>
+  <si>
     <t xml:space="preserve">Cladiella</t>
   </si>
   <si>
@@ -1348,6 +1366,9 @@
     <t xml:space="preserve">Echinopora lamellosa</t>
   </si>
   <si>
+    <t xml:space="preserve">Echinopora mammiformis</t>
+  </si>
+  <si>
     <t xml:space="preserve">Echinothrix</t>
   </si>
   <si>
@@ -1753,6 +1774,9 @@
     <t xml:space="preserve">Lithophyllon</t>
   </si>
   <si>
+    <t xml:space="preserve">Lithothamnion</t>
+  </si>
+  <si>
     <t xml:space="preserve">Litophyton</t>
   </si>
   <si>
@@ -1840,6 +1864,9 @@
     <t xml:space="preserve">Martensia</t>
   </si>
   <si>
+    <t xml:space="preserve">Mastophora</t>
+  </si>
+  <si>
     <t xml:space="preserve">Meandrina</t>
   </si>
   <si>
@@ -1870,6 +1897,9 @@
     <t xml:space="preserve">Merulinidae</t>
   </si>
   <si>
+    <t xml:space="preserve">Mesophyllum</t>
+  </si>
+  <si>
     <t xml:space="preserve">Microbial mats</t>
   </si>
   <si>
@@ -2014,6 +2044,9 @@
     <t xml:space="preserve">Nemenzophyllia</t>
   </si>
   <si>
+    <t xml:space="preserve">Neogoniolithon</t>
+  </si>
+  <si>
     <t xml:space="preserve">Neomeris</t>
   </si>
   <si>
@@ -2044,9 +2077,15 @@
     <t xml:space="preserve">Nudibranch</t>
   </si>
   <si>
+    <t xml:space="preserve">Nutrient indicator algae</t>
+  </si>
+  <si>
     <t xml:space="preserve">Obscured</t>
   </si>
   <si>
+    <t xml:space="preserve">Oceana</t>
+  </si>
+  <si>
     <t xml:space="preserve">Oceana serrulata</t>
   </si>
   <si>
@@ -2371,6 +2410,9 @@
     <t xml:space="preserve">Poritidae</t>
   </si>
   <si>
+    <t xml:space="preserve">Porolithon</t>
+  </si>
+  <si>
     <t xml:space="preserve">Porolithon antillarum</t>
   </si>
   <si>
@@ -2437,6 +2479,9 @@
     <t xml:space="preserve">Raspailiidae</t>
   </si>
   <si>
+    <t xml:space="preserve">Recently killed coral</t>
+  </si>
+  <si>
     <t xml:space="preserve">Reef matrix</t>
   </si>
   <si>
@@ -2488,6 +2533,9 @@
     <t xml:space="preserve">Ruppia maritima</t>
   </si>
   <si>
+    <t xml:space="preserve">Sabellidae</t>
+  </si>
+  <si>
     <t xml:space="preserve">Sand</t>
   </si>
   <si>
@@ -2512,10 +2560,7 @@
     <t xml:space="preserve">Sargassum hystrix</t>
   </si>
   <si>
-    <t xml:space="preserve">Scapophyllia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Scapophyllia cylindrica</t>
+    <t xml:space="preserve">Schizothrix</t>
   </si>
   <si>
     <t xml:space="preserve">Scleractinia</t>
@@ -2560,6 +2605,9 @@
     <t xml:space="preserve">Seriatopora hystrix</t>
   </si>
   <si>
+    <t xml:space="preserve">Serpulidae</t>
+  </si>
+  <si>
     <t xml:space="preserve">Siderastrea</t>
   </si>
   <si>
@@ -2692,6 +2740,9 @@
     <t xml:space="preserve">tire</t>
   </si>
   <si>
+    <t xml:space="preserve">Titanoderma</t>
+  </si>
+  <si>
     <t xml:space="preserve">Trachyphyllia</t>
   </si>
   <si>
@@ -2807,6 +2858,9 @@
   </si>
   <si>
     <t xml:space="preserve">Zoanthid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zoanthidae</t>
   </si>
   <si>
     <t xml:space="preserve">Zoopilus</t>
@@ -7109,6 +7163,96 @@
         <v>932</v>
       </c>
     </row>
+    <row r="757">
+      <c r="A757" t="s">
+        <v>933</v>
+      </c>
+    </row>
+    <row r="758">
+      <c r="A758" t="s">
+        <v>934</v>
+      </c>
+    </row>
+    <row r="759">
+      <c r="A759" t="s">
+        <v>935</v>
+      </c>
+    </row>
+    <row r="760">
+      <c r="A760" t="s">
+        <v>936</v>
+      </c>
+    </row>
+    <row r="761">
+      <c r="A761" t="s">
+        <v>937</v>
+      </c>
+    </row>
+    <row r="762">
+      <c r="A762" t="s">
+        <v>938</v>
+      </c>
+    </row>
+    <row r="763">
+      <c r="A763" t="s">
+        <v>939</v>
+      </c>
+    </row>
+    <row r="764">
+      <c r="A764" t="s">
+        <v>940</v>
+      </c>
+    </row>
+    <row r="765">
+      <c r="A765" t="s">
+        <v>941</v>
+      </c>
+    </row>
+    <row r="766">
+      <c r="A766" t="s">
+        <v>942</v>
+      </c>
+    </row>
+    <row r="767">
+      <c r="A767" t="s">
+        <v>943</v>
+      </c>
+    </row>
+    <row r="768">
+      <c r="A768" t="s">
+        <v>944</v>
+      </c>
+    </row>
+    <row r="769">
+      <c r="A769" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="770">
+      <c r="A770" t="s">
+        <v>946</v>
+      </c>
+    </row>
+    <row r="771">
+      <c r="A771" t="s">
+        <v>947</v>
+      </c>
+    </row>
+    <row r="772">
+      <c r="A772" t="s">
+        <v>948</v>
+      </c>
+    </row>
+    <row r="773">
+      <c r="A773" t="s">
+        <v>949</v>
+      </c>
+    </row>
+    <row r="774">
+      <c r="A774" t="s">
+        <v>950</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
@@ -7125,57 +7269,57 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>934</v>
+        <v>952</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>935</v>
+        <v>953</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>936</v>
+        <v>954</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>937</v>
+        <v>955</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>938</v>
+        <v>956</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>939</v>
+        <v>957</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>940</v>
+        <v>958</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>941</v>
+        <v>959</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>942</v>
+        <v>960</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>943</v>
+        <v>961</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>944</v>
+        <v>962</v>
       </c>
     </row>
   </sheetData>
@@ -7467,7 +7611,7 @@
         <v>140</v>
       </c>
       <c r="C25" t="s">
-        <v>933</v>
+        <v>951</v>
       </c>
     </row>
     <row r="26">
@@ -7478,7 +7622,7 @@
         <v>28</v>
       </c>
       <c r="C26" t="s">
-        <v>945</v>
+        <v>963</v>
       </c>
     </row>
   </sheetData>

</xml_diff>